<commit_message>
added more classes, basic features are complete, only missing spells now
</commit_message>
<xml_diff>
--- a/classes.xlsx
+++ b/classes.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\WebApps\rgcconsole\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938AB7E9-EDD7-45AB-989F-D35EECDF2269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD72876-3782-43AB-AE79-D1D3704A4831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DF87F495-21D1-48FB-92CA-A3B7B4FE80E8}"/>
   </bookViews>
   <sheets>
     <sheet name="class examples" sheetId="1" r:id="rId1"/>
     <sheet name="weights" sheetId="2" r:id="rId2"/>
+    <sheet name="defaultSkill" sheetId="3" r:id="rId3"/>
+    <sheet name="barbarian" sheetId="4" r:id="rId4"/>
+    <sheet name="scout" sheetId="5" r:id="rId5"/>
+    <sheet name="knight" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="76">
   <si>
     <t>class</t>
   </si>
@@ -139,6 +143,129 @@
   </si>
   <si>
     <t>money-points ratio</t>
+  </si>
+  <si>
+    <t>FantasySkills.Academia</t>
+  </si>
+  <si>
+    <t>FantasySkills.Acrobatics</t>
+  </si>
+  <si>
+    <t>FantasySkills.Administration</t>
+  </si>
+  <si>
+    <t>FantasySkills.AnimalHandling</t>
+  </si>
+  <si>
+    <t>FantasySkills.Athletics</t>
+  </si>
+  <si>
+    <t>FantasySkills.Craft</t>
+  </si>
+  <si>
+    <t>FantasySkills.Engineering</t>
+  </si>
+  <si>
+    <t>FantasySkills.Singing</t>
+  </si>
+  <si>
+    <t>FantasySkills.Dancing</t>
+  </si>
+  <si>
+    <t>FantasySkills.Sculpting</t>
+  </si>
+  <si>
+    <t>FantasySkills.Music</t>
+  </si>
+  <si>
+    <t>FantasySkills.Storytelling</t>
+  </si>
+  <si>
+    <t>FantasySkills.Puppetry</t>
+  </si>
+  <si>
+    <t>FantasySkills.Painting</t>
+  </si>
+  <si>
+    <t>FantasySkills.Humanities</t>
+  </si>
+  <si>
+    <t>FantasySkills.Intrusion</t>
+  </si>
+  <si>
+    <t>FantasySkills.Investigation</t>
+  </si>
+  <si>
+    <t>FantasySkills.Medicine</t>
+  </si>
+  <si>
+    <t>FantasySkills.Meditation</t>
+  </si>
+  <si>
+    <t>FantasySkills.Mysticism</t>
+  </si>
+  <si>
+    <t>FantasySkills.Persuasion</t>
+  </si>
+  <si>
+    <t>FantasySkills.Psychology</t>
+  </si>
+  <si>
+    <t>FantasySkills.ScienceAlchemy</t>
+  </si>
+  <si>
+    <t>FantasySkills.ScienceMathematics</t>
+  </si>
+  <si>
+    <t>FantasySkills.ScienceAstronomy</t>
+  </si>
+  <si>
+    <t>FantasySkills.ScienceNature</t>
+  </si>
+  <si>
+    <t>FantasySkills.ScienceGeology</t>
+  </si>
+  <si>
+    <t>FantasySkills.Stealth</t>
+  </si>
+  <si>
+    <t>FantasySkills.Streetwise</t>
+  </si>
+  <si>
+    <t>FantasySkills.Survival</t>
+  </si>
+  <si>
+    <t>FantasySkills.Tactics</t>
+  </si>
+  <si>
+    <t>FantasySkills.Trickery</t>
+  </si>
+  <si>
+    <t>FantasySkills.Vehicle</t>
+  </si>
+  <si>
+    <t>CombatSkills.Archery</t>
+  </si>
+  <si>
+    <t>CombatSkills.BladedWeapon</t>
+  </si>
+  <si>
+    <t>CombatSkills.BluntWeapon</t>
+  </si>
+  <si>
+    <t>CombatSkills.Crossbows</t>
+  </si>
+  <si>
+    <t>CombatSkills.Firearms</t>
+  </si>
+  <si>
+    <t>CombatSkills.Shield</t>
+  </si>
+  <si>
+    <t>CombatSkills.UnarmedStrikes</t>
+  </si>
+  <si>
+    <t>CombatSKills.Wrestling</t>
   </si>
 </sst>
 </file>
@@ -1053,7 +1180,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,4 +1762,1402 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE476FF2-A56E-4349-99EF-D582BBC3C37D}">
+  <dimension ref="A1:B41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A29" sqref="A1:B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E23C81D8-DEAF-4F2B-B761-21AF2E8EE3F6}">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1">
+        <v>-0.01</v>
+      </c>
+      <c r="D1">
+        <f>SUM(B1:B41)</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5402FD6-4CE2-4C52-8B3F-77F489F63F13}">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1">
+        <v>-0.01</v>
+      </c>
+      <c r="D1">
+        <f>SUM(B1:B41)</f>
+        <v>0.22600000000000006</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D8E201-E06C-4703-9336-063CA86DBD96}">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <f>SUM(B1:B41)</f>
+        <v>0.28300000000000003</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41">
+        <v>0.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>